<commit_message>
Update: ppt 자동 생성 구현
</commit_message>
<xml_diff>
--- a/tests/test_data/sample_birthday.xlsx
+++ b/tests/test_data/sample_birthday.xlsx
@@ -52,19 +52,19 @@
     <t>1990-01-15</t>
   </si>
   <si>
-    <t>1992-03-22</t>
+    <t>1992-01-22</t>
   </si>
   <si>
     <t>1988-01-30</t>
   </si>
   <si>
-    <t>1995-06-18</t>
-  </si>
-  <si>
-    <t>1993-03-05</t>
-  </si>
-  <si>
-    <t>1991-09-10</t>
+    <t>1995-01-18</t>
+  </si>
+  <si>
+    <t>1993-01-05</t>
+  </si>
+  <si>
+    <t>1991-01-10</t>
   </si>
 </sst>
 </file>

</xml_diff>